<commit_message>
commit : Aug 25
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/hs/keyword/scenarios/Avesdo_Test_scenarios.xlsx
+++ b/src/main/java/com/qa/hs/keyword/scenarios/Avesdo_Test_scenarios.xlsx
@@ -119,7 +119,7 @@
     <t xml:space="preserve">sendKeys</t>
   </si>
   <si>
-    <t xml:space="preserve">AAAAAAExample</t>
+    <t xml:space="preserve">AABHIExample</t>
   </si>
   <si>
     <t xml:space="preserve">select title</t>
@@ -566,8 +566,8 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Aug 30 : commit
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/hs/keyword/scenarios/Avesdo_Test_scenarios.xlsx
+++ b/src/main/java/com/qa/hs/keyword/scenarios/Avesdo_Test_scenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="118">
   <si>
     <t xml:space="preserve">test step</t>
   </si>
@@ -293,9 +293,6 @@
   </si>
   <si>
     <t xml:space="preserve">//div[@data-value='No']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">w</t>
   </si>
   <si>
     <t xml:space="preserve">click SALES</t>
@@ -480,7 +477,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -503,10 +500,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -595,12 +588,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.0222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.2740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.5555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.4703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.0037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.8074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.4481481481482"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.6444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -711,18 +704,18 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.537037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="102.307407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.1259259259259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="104.951851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -773,7 +766,7 @@
       <c r="D3" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="0" t="n">
         <v>3000</v>
       </c>
     </row>
@@ -1110,10 +1103,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.262962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.6111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.9481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.5888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1376,16 +1369,16 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.52592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.7814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.9592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1436,19 +1429,19 @@
       <c r="D3" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>90</v>
+      <c r="E3" s="0" t="n">
+        <v>3000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>92</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>20</v>
@@ -1459,13 +1452,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>94</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>20</v>
@@ -1476,13 +1469,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>96</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>20</v>
@@ -1493,13 +1486,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>98</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>20</v>
@@ -1510,30 +1503,30 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>100</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>103</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>20</v>
@@ -1544,13 +1537,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>105</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>20</v>
@@ -1561,13 +1554,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>106</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>20</v>
@@ -1578,19 +1571,19 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>109</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>31</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,13 +1594,13 @@
         <v>18</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1618,24 +1611,24 @@
         <v>18</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>115</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>116</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>20</v>
@@ -1657,19 +1650,19 @@
       <c r="D16" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>90</v>
+      <c r="E16" s="0" t="n">
+        <v>2000</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>117</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>118</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
commit : sep 10
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/hs/keyword/scenarios/Avesdo_Test_scenarios.xlsx
+++ b/src/main/java/com/qa/hs/keyword/scenarios/Avesdo_Test_scenarios.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="139">
   <si>
     <t xml:space="preserve">test step</t>
   </si>
@@ -388,7 +388,7 @@
     <t xml:space="preserve">click available home</t>
   </si>
   <si>
-    <t xml:space="preserve">(//div[@style='color: rgb(255, 255, 255);'])[1]</t>
+    <t xml:space="preserve">(//div[@status='Available'])[1]</t>
   </si>
   <si>
     <t xml:space="preserve">click allocate unit</t>
@@ -412,52 +412,34 @@
     <t xml:space="preserve">(//span[@class='mat-option-text'])[2]</t>
   </si>
   <si>
-    <t xml:space="preserve">click on select a puchaser</t>
+    <t xml:space="preserve">enter purchaser</t>
   </si>
   <si>
     <t xml:space="preserve">//input[@placeholder='Select a Purchaser']</t>
   </si>
   <si>
-    <t xml:space="preserve">click on add new purchaser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//span[normalize-space()='Add New Purchaser']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enter first name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">//input[@data-placeholder='First name']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PurchaserExample</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//input[@data-placeholder='Last name']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lastName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//input[@data-placeholder='Email']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tghyu@sdf.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">click add purchaser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(//span[normalize-space()='Add Purchaser'])[2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//span[@class='mat-checkbox-inner-container']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">click No time restriction checkbox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//span[normalize-space()='SUBMIT']</t>
+    <t xml:space="preserve">select a purchaser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">click </t>
+  </si>
+  <si>
+    <t xml:space="preserve">//input[@formcontrolname='hour']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enter hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(//span[normalize-space()='SUBMIT'])[2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">click jse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">click continue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//button[normalize-space()='Continue']</t>
   </si>
 </sst>
 </file>
@@ -669,12 +651,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.3148148148148"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.2185185185185"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.5259259259259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.4555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.6222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.0777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.1703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.3148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -791,12 +773,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="118.962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.1481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="125.137037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.9333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1201,10 +1183,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.7814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,18 +1685,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.937037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.5814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1820,7 +1802,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>120</v>
       </c>
@@ -1888,7 +1870,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>129</v>
       </c>
@@ -1899,13 +1881,13 @@
         <v>130</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>131</v>
       </c>
@@ -1913,78 +1895,78 @@
         <v>18</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="E12" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="B14" s="0" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E14" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>138</v>
+        <v>6</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>139</v>
+        <v>26</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>3000</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>6</v>
@@ -1992,76 +1974,39 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>56</v>
+        <v>137</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>142</v>
+        <v>6</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="0" t="n">
+      <c r="E18" s="0" t="n">
         <v>2000</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E15" r:id="rId1" display="tghyu@sdf.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>